<commit_message>
Added updated positions and bootleg test for sequencing
</commit_message>
<xml_diff>
--- a/robotcontrol/RobotPositions.xlsx
+++ b/robotcontrol/RobotPositions.xlsx
@@ -1619,8 +1619,8 @@
       <c r="G11" t="s" s="11">
         <v>18</v>
       </c>
-      <c r="H11" t="s" s="11">
-        <v>18</v>
+      <c r="H11" s="10">
+        <v>275</v>
       </c>
     </row>
     <row r="12" ht="20.35" customHeight="1">
@@ -1643,8 +1643,8 @@
       <c r="G12" t="s" s="11">
         <v>18</v>
       </c>
-      <c r="H12" t="s" s="11">
-        <v>18</v>
+      <c r="H12" s="10">
+        <v>425</v>
       </c>
     </row>
     <row r="13" ht="20.35" customHeight="1">

</xml_diff>

<commit_message>
int conversion and nan checking
</commit_message>
<xml_diff>
--- a/robotcontrol/RobotPositions.xlsx
+++ b/robotcontrol/RobotPositions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Table 1</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>grip_open</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t>grip_closed</t>
@@ -241,7 +238,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -273,9 +270,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1604,54 +1598,34 @@
         <v>17</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s" s="11">
-        <v>18</v>
-      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="10">
         <v>275</v>
       </c>
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="A12" t="s" s="7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="E12" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="G12" t="s" s="11">
-        <v>18</v>
-      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="10">
         <v>425</v>
       </c>
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="B13" s="12">
+        <v>19</v>
+      </c>
+      <c r="B13" s="11">
         <v>1</v>
       </c>
       <c r="C13" s="10">
@@ -1674,7 +1648,7 @@
       </c>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="13"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1684,7 +1658,7 @@
       <c r="H14" s="9"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="13"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1694,7 +1668,7 @@
       <c r="H15" s="9"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="13"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1704,7 +1678,7 @@
       <c r="H16" s="9"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="13"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1714,7 +1688,7 @@
       <c r="H17" s="9"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="13"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1724,7 +1698,7 @@
       <c r="H18" s="9"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="13"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>

</xml_diff>

<commit_message>
added RPI specifics back in for testing
</commit_message>
<xml_diff>
--- a/robotcontrol/RobotPositions.xlsx
+++ b/robotcontrol/RobotPositions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Table 1</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>safety</t>
+  </si>
+  <si>
+    <t>rest</t>
   </si>
 </sst>
 </file>
@@ -1648,11 +1651,19 @@
       </c>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="12"/>
+      <c r="A14" t="s" s="7">
+        <v>20</v>
+      </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="10">
+        <v>500</v>
+      </c>
+      <c r="D14" s="10">
+        <v>150</v>
+      </c>
+      <c r="E14" s="10">
+        <v>340</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>

</xml_diff>

<commit_message>
updated spreadsheet for new structure
</commit_message>
<xml_diff>
--- a/robotcontrol/RobotPositions.xlsx
+++ b/robotcontrol/RobotPositions.xlsx
@@ -6,16 +6,14 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Teachpoints" sheetId="1" r:id="rId4"/>
+    <sheet name="Sequences" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Position</t>
   </si>
@@ -75,6 +73,30 @@
   </si>
   <si>
     <t>rest</t>
+  </si>
+  <si>
+    <t>sequence</t>
+  </si>
+  <si>
+    <t>teachpoints</t>
+  </si>
+  <si>
+    <t>delays</t>
+  </si>
+  <si>
+    <t>loop</t>
+  </si>
+  <si>
+    <t>Pick_Place_cups</t>
+  </si>
+  <si>
+    <t>safety, left_pick_hover, left_pick, grip_closed, left_pick_hover, right_pick_hover, grip_open, right_pick</t>
+  </si>
+  <si>
+    <t>1,1,1,1,1,1,1,1</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -241,15 +263,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -279,6 +298,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1395,10 +1426,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1414,315 +1445,410 @@
     <col min="9" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
+    <row r="1" ht="20.55" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="20.55" customHeight="1">
       <c r="A2" t="s" s="3">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" ht="20.35" customHeight="1">
+      <c r="A3" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="A4" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="9">
+        <v>400</v>
+      </c>
+      <c r="D4" s="9">
+        <v>300</v>
+      </c>
+      <c r="E4" s="9">
+        <v>450</v>
+      </c>
+      <c r="F4" s="9">
+        <v>525</v>
+      </c>
+      <c r="G4" s="9">
+        <v>340</v>
+      </c>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" ht="20.35" customHeight="1">
+      <c r="A5" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="9">
+        <v>400</v>
+      </c>
+      <c r="D5" s="9">
+        <v>400</v>
+      </c>
+      <c r="E5" s="9">
+        <v>450</v>
+      </c>
+      <c r="F5" s="9">
+        <v>610</v>
+      </c>
+      <c r="G5" s="9">
+        <v>340</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" ht="20.35" customHeight="1">
+      <c r="A6" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" ht="20.35" customHeight="1">
+      <c r="A7" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" ht="20.35" customHeight="1">
+      <c r="A8" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="9">
+        <v>500</v>
+      </c>
+      <c r="D8" s="9">
+        <v>300</v>
+      </c>
+      <c r="E8" s="9">
+        <v>450</v>
+      </c>
+      <c r="F8" s="9">
+        <v>525</v>
+      </c>
+      <c r="G8" s="9">
+        <v>340</v>
+      </c>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" ht="20.35" customHeight="1">
+      <c r="A9" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="9">
+        <v>500</v>
+      </c>
+      <c r="D9" s="9">
+        <v>400</v>
+      </c>
+      <c r="E9" s="9">
+        <v>450</v>
+      </c>
+      <c r="F9" s="9">
+        <v>610</v>
+      </c>
+      <c r="G9" s="9">
+        <v>340</v>
+      </c>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" ht="20.35" customHeight="1">
+      <c r="A10" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" ht="20.35" customHeight="1">
+      <c r="A11" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="12" ht="20.35" customHeight="1">
+      <c r="A12" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="B12" s="10">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="3">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="C12" s="9">
+        <v>500</v>
+      </c>
+      <c r="D12" s="9">
+        <v>250</v>
+      </c>
+      <c r="E12" s="9">
+        <v>400</v>
+      </c>
+      <c r="F12" s="9">
+        <v>525</v>
+      </c>
+      <c r="G12" s="9">
+        <v>340</v>
+      </c>
+      <c r="H12" s="9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" ht="20.35" customHeight="1">
+      <c r="A13" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="9">
+        <v>500</v>
+      </c>
+      <c r="D13" s="9">
+        <v>150</v>
+      </c>
+      <c r="E13" s="9">
+        <v>340</v>
+      </c>
+      <c r="F13" s="9">
+        <v>700</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" ht="20.35" customHeight="1">
+      <c r="A14" s="11"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" ht="20.35" customHeight="1">
+      <c r="A15" s="11"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" ht="20.35" customHeight="1">
+      <c r="A16" s="11"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" ht="20.35" customHeight="1">
+      <c r="A17" s="11"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" ht="20.35" customHeight="1">
+      <c r="A18" s="11"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="16.3516" style="12" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="12" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="12" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20.55" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" ht="104.55" customHeight="1">
+      <c r="A2" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s" s="15">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" ht="20.35" customHeight="1">
+      <c r="A3" s="11"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10">
-        <v>400</v>
-      </c>
-      <c r="D5" s="10">
-        <v>300</v>
-      </c>
-      <c r="E5" s="10">
-        <v>450</v>
-      </c>
-      <c r="F5" s="10">
-        <v>525</v>
-      </c>
-      <c r="G5" s="10">
-        <v>340</v>
-      </c>
-      <c r="H5" s="10">
-        <v>275</v>
-      </c>
+      <c r="A5" s="11"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10">
-        <v>400</v>
-      </c>
-      <c r="D6" s="10">
-        <v>400</v>
-      </c>
-      <c r="E6" s="10">
-        <v>450</v>
-      </c>
-      <c r="F6" s="10">
-        <v>610</v>
-      </c>
-      <c r="G6" s="10">
-        <v>340</v>
-      </c>
-      <c r="H6" s="10">
-        <v>275</v>
-      </c>
+      <c r="A6" s="11"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>13</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="10">
-        <v>500</v>
-      </c>
-      <c r="D9" s="10">
-        <v>300</v>
-      </c>
-      <c r="E9" s="10">
-        <v>450</v>
-      </c>
-      <c r="F9" s="10">
-        <v>525</v>
-      </c>
-      <c r="G9" s="10">
-        <v>340</v>
-      </c>
-      <c r="H9" s="10">
-        <v>275</v>
-      </c>
+      <c r="A9" s="11"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10">
-        <v>500</v>
-      </c>
-      <c r="D10" s="10">
-        <v>400</v>
-      </c>
-      <c r="E10" s="10">
-        <v>450</v>
-      </c>
-      <c r="F10" s="10">
-        <v>610</v>
-      </c>
-      <c r="G10" s="10">
-        <v>340</v>
-      </c>
-      <c r="H10" s="10">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B13" s="11">
-        <v>1</v>
-      </c>
-      <c r="C13" s="10">
-        <v>500</v>
-      </c>
-      <c r="D13" s="10">
-        <v>250</v>
-      </c>
-      <c r="E13" s="10">
-        <v>400</v>
-      </c>
-      <c r="F13" s="10">
-        <v>525</v>
-      </c>
-      <c r="G13" s="10">
-        <v>340</v>
-      </c>
-      <c r="H13" s="10">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="10">
-        <v>500</v>
-      </c>
-      <c r="D14" s="10">
-        <v>150</v>
-      </c>
-      <c r="E14" s="10">
-        <v>340</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>

</xml_diff>

<commit_message>
Added functional dataposter class
</commit_message>
<xml_diff>
--- a/robotcontrol/RobotPositions.xlsx
+++ b/robotcontrol/RobotPositions.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Position</t>
   </si>
@@ -93,7 +93,10 @@
     <t>1,1,1,1,1,1,1,1</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Spinmove</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -246,13 +249,43 @@
         <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -271,7 +304,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -311,7 +344,16 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1782,16 +1824,24 @@
       <c r="C2" t="s" s="12">
         <v>25</v>
       </c>
-      <c r="D2" t="s" s="12">
+      <c r="D2" t="s" s="13">
         <v>26</v>
       </c>
-      <c r="E2" s="13"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s" s="15">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s" s="13">
+        <v>25</v>
+      </c>
+      <c r="D3" t="b" s="16">
+        <v>0</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">

</xml_diff>